<commit_message>
Module 5. Task 1. Updated docs. Task 2. Added todo list.
</commit_message>
<xml_diff>
--- a/Module5/Task 1/Performance measurement.xlsx
+++ b/Module5/Task 1/Performance measurement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="4695" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Insert (seconds)</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>50K repeats</t>
+  </si>
+  <si>
+    <t>With cache</t>
   </si>
 </sst>
 </file>
@@ -304,6 +307,9 @@
               <c:f>Sheet1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>With cache</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -385,6 +391,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>124.40633939999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.208470000000005</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1549,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R35" sqref="R35"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1589,6 +1601,17 @@
         <v>213.31347550000001</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>124.40633939999999</v>
+      </c>
+      <c r="C3">
+        <v>93.208470000000005</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>